<commit_message>
Added missing regex for 'clustering_resolution' in the 'regex_to_formula' field; Updated schema version to 0.3
</commit_message>
<xml_diff>
--- a/single_cell/singlecell_schema_main_v0.3.xlsx
+++ b/single_cell/singlecell_schema_main_v0.3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10727"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zef22hak/development/COPO-schemas/single_cell/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/providen/Documents/EI/Projects/SingleCellSchemas/schemas/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9BD1A46-EF6B-E44C-A1F5-C2798A813291}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03876C63-4DA1-6B4C-8BD5-CA9C2EB6D3D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{7BD8D0E6-E1F4-E04F-9790-31602B31B6DB}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17960" xr2:uid="{7BD8D0E6-E1F4-E04F-9790-31602B31B6DB}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -81,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4532" uniqueCount="1900">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4534" uniqueCount="1902">
   <si>
     <t>component_name</t>
   </si>
@@ -5907,6 +5907,12 @@
   </si>
   <si>
     <t>expression_data_file_checksum</t>
+  </si>
+  <si>
+    <t>^([0-9]*[.])?[0-9]+</t>
+  </si>
+  <si>
+    <t>AND(ISNUMBER(VALUE({column_letter}{row_start})), VALUE({column_letter}{row_start}) &gt;= 0)</t>
   </si>
 </sst>
 </file>
@@ -6088,7 +6094,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="68">
+  <borders count="69">
     <border>
       <left/>
       <right/>
@@ -6939,12 +6945,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="163">
+  <cellXfs count="166">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -7404,6 +7425,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="68" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="68" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -7782,12 +7810,12 @@
   <sheetPr>
     <tabColor theme="5" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="A1:X222"/>
+  <dimension ref="A1:X223"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A175" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="4" topLeftCell="E1" activePane="topRight" state="frozen"/>
       <selection activeCell="A23" sqref="A23"/>
-      <selection pane="topRight" activeCell="C217" sqref="C217"/>
+      <selection pane="topRight" activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" customHeight="1"/>
@@ -19428,7 +19456,7 @@
       <c r="W211" s="40"/>
       <c r="X211" s="72"/>
     </row>
-    <row r="212" spans="1:24" s="160" customFormat="1" ht="15.75" customHeight="1" thickTop="1" thickBot="1">
+    <row r="212" spans="1:24" s="160" customFormat="1" ht="15.75" customHeight="1" thickTop="1">
       <c r="A212" s="160" t="s">
         <v>822</v>
       </c>
@@ -19491,8 +19519,8 @@
       <c r="W212" s="158"/>
       <c r="X212" s="159"/>
     </row>
-    <row r="213" spans="1:24" ht="15.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A213" s="160" t="s">
+    <row r="213" spans="1:24" ht="15.75" customHeight="1">
+      <c r="A213" s="165" t="s">
         <v>822</v>
       </c>
       <c r="B213" s="3" t="s">
@@ -19553,8 +19581,8 @@
       <c r="W213" s="33"/>
       <c r="X213" s="71"/>
     </row>
-    <row r="214" spans="1:24" ht="15.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A214" s="160" t="s">
+    <row r="214" spans="1:24" ht="15.75" customHeight="1">
+      <c r="A214" s="165" t="s">
         <v>822</v>
       </c>
       <c r="B214" s="3" t="s">
@@ -19615,8 +19643,8 @@
       <c r="W214" s="14"/>
       <c r="X214" s="68"/>
     </row>
-    <row r="215" spans="1:24" ht="15.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A215" s="160" t="s">
+    <row r="215" spans="1:24" ht="15.75" customHeight="1">
+      <c r="A215" s="165" t="s">
         <v>822</v>
       </c>
       <c r="B215" s="3" t="s">
@@ -19674,8 +19702,8 @@
       <c r="W215" s="14"/>
       <c r="X215" s="68"/>
     </row>
-    <row r="216" spans="1:24" ht="15.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A216" s="160" t="s">
+    <row r="216" spans="1:24" ht="15.75" customHeight="1">
+      <c r="A216" s="165" t="s">
         <v>822</v>
       </c>
       <c r="B216" s="3" t="s">
@@ -19724,8 +19752,8 @@
       <c r="W216" s="14"/>
       <c r="X216" s="68"/>
     </row>
-    <row r="217" spans="1:24" ht="15.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A217" s="160" t="s">
+    <row r="217" spans="1:24" ht="15.75" customHeight="1">
+      <c r="A217" s="165" t="s">
         <v>822</v>
       </c>
       <c r="B217" s="3" t="s">
@@ -19777,8 +19805,8 @@
       <c r="W217" s="14"/>
       <c r="X217" s="68"/>
     </row>
-    <row r="218" spans="1:24" ht="15.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A218" s="160" t="s">
+    <row r="218" spans="1:24" ht="15.75" customHeight="1">
+      <c r="A218" s="165" t="s">
         <v>822</v>
       </c>
       <c r="B218" s="3" t="s">
@@ -19827,8 +19855,8 @@
       <c r="W218" s="14"/>
       <c r="X218" s="68"/>
     </row>
-    <row r="219" spans="1:24" ht="15.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A219" s="160" t="s">
+    <row r="219" spans="1:24" ht="15.75" customHeight="1">
+      <c r="A219" s="165" t="s">
         <v>822</v>
       </c>
       <c r="B219" s="3" t="s">
@@ -19883,8 +19911,8 @@
       <c r="W219" s="14"/>
       <c r="X219" s="68"/>
     </row>
-    <row r="220" spans="1:24" ht="15.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A220" s="160" t="s">
+    <row r="220" spans="1:24" ht="15.75" customHeight="1">
+      <c r="A220" s="165" t="s">
         <v>822</v>
       </c>
       <c r="B220" s="3" t="s">
@@ -19939,8 +19967,8 @@
       <c r="W220" s="14"/>
       <c r="X220" s="68"/>
     </row>
-    <row r="221" spans="1:24" ht="15.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A221" s="160" t="s">
+    <row r="221" spans="1:24" ht="15.75" customHeight="1">
+      <c r="A221" s="165" t="s">
         <v>822</v>
       </c>
       <c r="B221" s="3" t="s">
@@ -19995,8 +20023,8 @@
       <c r="W221" s="14"/>
       <c r="X221" s="68"/>
     </row>
-    <row r="222" spans="1:24" ht="15.75" customHeight="1" thickTop="1">
-      <c r="A222" s="160" t="s">
+    <row r="222" spans="1:24" ht="15.75" customHeight="1">
+      <c r="A222" s="165" t="s">
         <v>822</v>
       </c>
       <c r="B222" s="3" t="s">
@@ -20053,6 +20081,9 @@
       <c r="V222" s="13"/>
       <c r="W222" s="14"/>
       <c r="X222" s="68"/>
+    </row>
+    <row r="223" spans="1:24" ht="15.75" customHeight="1">
+      <c r="A223" s="165"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:X195" xr:uid="{545CA0C1-0282-3A43-9C60-512DE414A571}"/>
@@ -39596,10 +39627,10 @@
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:I59"/>
+  <dimension ref="A1:I60"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="B60" sqref="B60"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
@@ -40179,21 +40210,31 @@
       <c r="C57" s="83"/>
     </row>
     <row r="58" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A58" s="55" t="s">
+      <c r="A58" s="82" t="s">
         <v>1764</v>
       </c>
-      <c r="B58" s="55" t="s">
+      <c r="B58" s="82" t="s">
         <v>1765</v>
       </c>
-      <c r="C58" s="56"/>
+      <c r="C58" s="83"/>
     </row>
     <row r="59" spans="1:3" ht="34">
-      <c r="A59" s="53" t="s">
+      <c r="A59" s="163" t="s">
         <v>180</v>
       </c>
-      <c r="B59" s="53" t="s">
+      <c r="B59" s="163" t="s">
         <v>1785</v>
       </c>
+      <c r="C59" s="164"/>
+    </row>
+    <row r="60" spans="1:3" ht="17">
+      <c r="A60" s="163" t="s">
+        <v>1900</v>
+      </c>
+      <c r="B60" s="163" t="s">
+        <v>1901</v>
+      </c>
+      <c r="C60" s="164"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:C53" xr:uid="{D95B3E19-31EE-401E-8E14-DBEF7BC74F95}"/>

</xml_diff>